<commit_message>
Refactor data preparation and file handling
</commit_message>
<xml_diff>
--- a/model/excel_sheets/Gender_10.xlsx
+++ b/model/excel_sheets/Gender_10.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,277 +436,212 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>Images</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Images</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
           <t>Gender</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>31791</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>data/img_align_celeba/031792.jpg</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>C:/Users/busse/Bachelorarbeit/CICD-Pipeline-Gender-Recognition/data/img_align_celeba\031792.jpg</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>126494</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>data/img_align_celeba/126495.jpg</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>C:/Users/busse/Bachelorarbeit/CICD-Pipeline-Gender-Recognition/data/img_align_celeba\126495.jpg</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>199367</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>data/img_align_celeba/199368.jpg</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>C:/Users/busse/Bachelorarbeit/CICD-Pipeline-Gender-Recognition/data/img_align_celeba\199368.jpg</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>46737</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>data/img_align_celeba/046738.jpg</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>C:/Users/busse/Bachelorarbeit/CICD-Pipeline-Gender-Recognition/data/img_align_celeba\046738.jpg</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>24240</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>data/img_align_celeba/024241.jpg</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>C:/Users/busse/Bachelorarbeit/CICD-Pipeline-Gender-Recognition/data/img_align_celeba\024241.jpg</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>98641</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>data/img_align_celeba/098642.jpg</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>C:/Users/busse/Bachelorarbeit/CICD-Pipeline-Gender-Recognition/data/img_align_celeba\098642.jpg</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>112330</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>data/img_align_celeba/112331.jpg</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>C:/Users/busse/Bachelorarbeit/CICD-Pipeline-Gender-Recognition/data/img_align_celeba\112331.jpg</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>71436</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>data/img_align_celeba/071437.jpg</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>C:/Users/busse/Bachelorarbeit/CICD-Pipeline-Gender-Recognition/data/img_align_celeba\071437.jpg</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>176927</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>data/img_align_celeba/176928.jpg</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>C:/Users/busse/Bachelorarbeit/CICD-Pipeline-Gender-Recognition/data/img_align_celeba\176928.jpg</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>61337</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>data/img_align_celeba/061338.jpg</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>C:/Users/busse/Bachelorarbeit/CICD-Pipeline-Gender-Recognition/data/img_align_celeba\061338.jpg</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>45514</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>data/img_align_celeba/045515.jpg</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>C:/Users/busse/Bachelorarbeit/CICD-Pipeline-Gender-Recognition/data/img_align_celeba\045515.jpg</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>38855</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>data/img_align_celeba/038856.jpg</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>C:/Users/busse/Bachelorarbeit/CICD-Pipeline-Gender-Recognition/data/img_align_celeba\038856.jpg</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>186393</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>data/img_align_celeba/186394.jpg</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>C:/Users/busse/Bachelorarbeit/CICD-Pipeline-Gender-Recognition/data/img_align_celeba\186394.jpg</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>147628</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>data/img_align_celeba/147629.jpg</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>C:/Users/busse/Bachelorarbeit/CICD-Pipeline-Gender-Recognition/data/img_align_celeba\147629.jpg</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>73633</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>data/img_align_celeba/073634.jpg</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>C:/Users/busse/Bachelorarbeit/CICD-Pipeline-Gender-Recognition/data/img_align_celeba\073634.jpg</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>135043</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>data/img_align_celeba/135044.jpg</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>C:/Users/busse/Bachelorarbeit/CICD-Pipeline-Gender-Recognition/data/img_align_celeba\135044.jpg</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>85971</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>data/img_align_celeba/085972.jpg</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>C:/Users/busse/Bachelorarbeit/CICD-Pipeline-Gender-Recognition/data/img_align_celeba\085972.jpg</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>171845</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>data/img_align_celeba/171846.jpg</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>C:/Users/busse/Bachelorarbeit/CICD-Pipeline-Gender-Recognition/data/img_align_celeba\171846.jpg</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>69846</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>data/img_align_celeba/069847.jpg</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>C:/Users/busse/Bachelorarbeit/CICD-Pipeline-Gender-Recognition/data/img_align_celeba\069847.jpg</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>198470</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>data/img_align_celeba/198471.jpg</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>C:/Users/busse/Bachelorarbeit/CICD-Pipeline-Gender-Recognition/data/img_align_celeba\198471.jpg</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add seaborn, tqdm, and scikit-learn dependencies
</commit_message>
<xml_diff>
--- a/model/excel_sheets/Gender_10.xlsx
+++ b/model/excel_sheets/Gender_10.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,278 +436,343 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>Images</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Images</t>
+          <t>Big_Nose</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>No_Beard</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>31791</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>data/img_align_celeba/031792.jpg</t>
         </is>
       </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>126494</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>data/img_align_celeba/126495.jpg</t>
         </is>
       </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>199367</v>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>data/img_align_celeba/199368.jpg</t>
         </is>
       </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
       <c r="C4" t="n">
         <v>1</v>
       </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>46737</v>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>data/img_align_celeba/046738.jpg</t>
         </is>
       </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>24240</v>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>data/img_align_celeba/024241.jpg</t>
         </is>
       </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>98641</v>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>data/img_align_celeba/098642.jpg</t>
         </is>
       </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>112330</v>
-      </c>
-      <c r="B8" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>data/img_align_celeba/112331.jpg</t>
         </is>
       </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
       <c r="C8" t="n">
         <v>1</v>
       </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>71436</v>
-      </c>
-      <c r="B9" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>data/img_align_celeba/071437.jpg</t>
         </is>
       </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>176927</v>
-      </c>
-      <c r="B10" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>data/img_align_celeba/176928.jpg</t>
         </is>
       </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
       <c r="C10" t="n">
         <v>1</v>
       </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>61337</v>
-      </c>
-      <c r="B11" t="inlineStr">
+      <c r="A11" t="inlineStr">
         <is>
           <t>data/img_align_celeba/061338.jpg</t>
         </is>
       </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
       <c r="C11" t="n">
         <v>1</v>
       </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>45514</v>
-      </c>
-      <c r="B12" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>data/img_align_celeba/045515.jpg</t>
         </is>
       </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
       <c r="C12" t="n">
         <v>1</v>
       </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>38855</v>
-      </c>
-      <c r="B13" t="inlineStr">
+      <c r="A13" t="inlineStr">
         <is>
           <t>data/img_align_celeba/038856.jpg</t>
         </is>
       </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>186393</v>
-      </c>
-      <c r="B14" t="inlineStr">
+      <c r="A14" t="inlineStr">
         <is>
           <t>data/img_align_celeba/186394.jpg</t>
         </is>
       </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>147628</v>
-      </c>
-      <c r="B15" t="inlineStr">
+      <c r="A15" t="inlineStr">
         <is>
           <t>data/img_align_celeba/147629.jpg</t>
         </is>
       </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
       <c r="C15" t="n">
         <v>1</v>
       </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>73633</v>
-      </c>
-      <c r="B16" t="inlineStr">
+      <c r="A16" t="inlineStr">
         <is>
           <t>data/img_align_celeba/073634.jpg</t>
         </is>
       </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>135043</v>
-      </c>
-      <c r="B17" t="inlineStr">
+      <c r="A17" t="inlineStr">
         <is>
           <t>data/img_align_celeba/135044.jpg</t>
         </is>
       </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
       <c r="C17" t="n">
         <v>1</v>
       </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>85971</v>
-      </c>
-      <c r="B18" t="inlineStr">
+      <c r="A18" t="inlineStr">
         <is>
           <t>data/img_align_celeba/085972.jpg</t>
         </is>
       </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>171845</v>
-      </c>
-      <c r="B19" t="inlineStr">
+      <c r="A19" t="inlineStr">
         <is>
           <t>data/img_align_celeba/171846.jpg</t>
         </is>
       </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
       <c r="C19" t="n">
         <v>1</v>
       </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>69846</v>
-      </c>
-      <c r="B20" t="inlineStr">
+      <c r="A20" t="inlineStr">
         <is>
           <t>data/img_align_celeba/069847.jpg</t>
         </is>
       </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
       <c r="C20" t="n">
         <v>1</v>
       </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>198470</v>
-      </c>
-      <c r="B21" t="inlineStr">
+      <c r="A21" t="inlineStr">
         <is>
           <t>data/img_align_celeba/198471.jpg</t>
         </is>
       </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
       <c r="C21" t="n">
         <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>